<commit_message>
expanding code for new samples
</commit_message>
<xml_diff>
--- a/TrueFlowValues_.xlsx
+++ b/TrueFlowValues_.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/625565b661b86efd/Documents/SeniorYear/MaterialsScience/flowability/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:1_{6B74AB0A-D348-454C-8B3F-66033CB1A7CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5A165EFD-BA85-5048-B05A-92F8C76C811E}"/>
+  <xr:revisionPtr revIDLastSave="262" documentId="13_ncr:1_{6B74AB0A-D348-454C-8B3F-66033CB1A7CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F7BCCFB0-EB0C-D744-AF6C-D2DABBAF71E7}"/>
   <bookViews>
-    <workbookView xWindow="17400" yWindow="460" windowWidth="22620" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13120" yWindow="460" windowWidth="22620" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Query1!$N$2:$N$9</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Query1!$N$2:$N$9</definedName>
     <definedName name="Query1">Query1!$A$1:$H$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="46">
   <si>
     <t>LotName</t>
   </si>
@@ -114,13 +116,70 @@
   </si>
   <si>
     <t>AugDensity</t>
+  </si>
+  <si>
+    <t>25-75</t>
+  </si>
+  <si>
+    <t>50-110</t>
+  </si>
+  <si>
+    <t>45-100</t>
+  </si>
+  <si>
+    <t>170-230</t>
+  </si>
+  <si>
+    <t>230-500</t>
+  </si>
+  <si>
+    <t>Valimet 1 Al F357.2</t>
+  </si>
+  <si>
+    <t>Valimet 2 AA 2024</t>
+  </si>
+  <si>
+    <t>Valimet 3 AA 4047</t>
+  </si>
+  <si>
+    <t>HC Stark TaH</t>
+  </si>
+  <si>
+    <t>HC Stark C103N 1st</t>
+  </si>
+  <si>
+    <t>HC Stark C103H</t>
+  </si>
+  <si>
+    <t>63-150</t>
+  </si>
+  <si>
+    <t>150-350</t>
+  </si>
+  <si>
+    <t>Valimet 4 Al P1015</t>
+  </si>
+  <si>
+    <t>Valimet 5 Al P1015</t>
+  </si>
+  <si>
+    <t>Valimet 6 Al P1015</t>
+  </si>
+  <si>
+    <t>HC Stark C103N 2nd</t>
+  </si>
+  <si>
+    <t>Ti-64</t>
+  </si>
+  <si>
+    <t>I-718</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +202,20 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -291,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -308,6 +381,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -323,6 +403,675 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{7B806548-0624-F141-9AA4-7509CBFC66E3}">
+          <cx:dataPt idx="0"/>
+          <cx:dataPt idx="1"/>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r">
+              <cx:binSize val="5"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39477EE4-2263-3842-9924-5F63C5C519F6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9461500" y="2559050"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -646,10 +1395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -664,7 +1413,7 @@
     <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -696,7 +1445,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>8</v>
       </c>
@@ -722,14 +1471,17 @@
         <v>26</v>
       </c>
       <c r="I2" s="11">
-        <f>IF(F2&gt;15, 1,0)</f>
+        <f>IF(F2&gt;12, 1,0)</f>
         <v>0</v>
       </c>
       <c r="J2" s="12">
         <v>4.657</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N2" s="11">
+        <v>3.78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
@@ -754,14 +1506,18 @@
       <c r="H3" s="8">
         <v>36</v>
       </c>
-      <c r="I3" s="8">
-        <v>2</v>
+      <c r="I3" s="11">
+        <f t="shared" ref="I3:I23" si="0">IF(F3&gt;12, 1,0)</f>
+        <v>1</v>
       </c>
       <c r="J3" s="13">
         <v>6.1150000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N3" s="3">
+        <v>34.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -786,14 +1542,18 @@
       <c r="H4" s="2">
         <v>30</v>
       </c>
-      <c r="I4" s="2">
-        <v>2</v>
+      <c r="I4" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="J4" s="14">
         <v>6.1150000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N4" s="2">
+        <v>26.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -818,14 +1578,18 @@
       <c r="H5" s="5">
         <v>31</v>
       </c>
-      <c r="I5" s="5">
-        <v>2</v>
+      <c r="I5" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="J5" s="15">
         <v>6.1150000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N5" s="8">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -850,14 +1614,18 @@
       <c r="H6" s="8">
         <v>33</v>
       </c>
-      <c r="I6" s="8">
-        <v>2</v>
+      <c r="I6" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="J6" s="13">
         <v>6.1150000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N6" s="8">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -882,14 +1650,18 @@
       <c r="H7" s="2">
         <v>29</v>
       </c>
-      <c r="I7" s="2">
-        <v>2</v>
+      <c r="I7" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="J7" s="14">
         <v>6.1150000000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N7" s="8">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
@@ -914,14 +1686,18 @@
       <c r="H8" s="5">
         <v>28</v>
       </c>
-      <c r="I8" s="5">
-        <v>2</v>
+      <c r="I8" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="J8" s="15">
         <v>6.1150000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N8" s="8">
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -946,15 +1722,18 @@
       <c r="H9" s="8">
         <v>29</v>
       </c>
-      <c r="I9" s="8">
-        <f t="shared" ref="I3:I23" si="0">IF(F9&gt;15, 1,0)</f>
+      <c r="I9" s="11">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J9" s="13">
         <v>5.9359999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N9" s="8">
+        <v>13.96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -979,7 +1758,7 @@
       <c r="H10" s="2">
         <v>26</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -987,7 +1766,7 @@
         <v>5.9359999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1012,7 +1791,7 @@
       <c r="H11" s="5">
         <v>28</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1020,7 +1799,7 @@
         <v>5.9359999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>17</v>
       </c>
@@ -1045,7 +1824,7 @@
       <c r="H12" s="8">
         <v>33</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1053,7 +1832,7 @@
         <v>5.9359999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1078,7 +1857,7 @@
       <c r="H13" s="2">
         <v>27</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1086,7 +1865,7 @@
         <v>5.9359999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
@@ -1111,7 +1890,7 @@
       <c r="H14" s="5">
         <v>27</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1119,7 +1898,7 @@
         <v>5.9359999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>18</v>
       </c>
@@ -1144,7 +1923,7 @@
       <c r="H15" s="8">
         <v>19</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1152,7 +1931,7 @@
         <v>7.6150000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1177,7 +1956,7 @@
       <c r="H16" s="2">
         <v>20</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1210,7 +1989,7 @@
       <c r="H17" s="5">
         <v>22</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1218,7 +1997,7 @@
         <v>7.6150000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>20</v>
       </c>
@@ -1243,14 +2022,15 @@
       <c r="H18" s="8">
         <v>24</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="11">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J18" s="13">
         <v>7.6150000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1275,7 +2055,8 @@
       <c r="H19" s="2">
         <v>20</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="11">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J19" s="14">
@@ -1307,14 +2088,15 @@
       <c r="H20" s="5">
         <v>19</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20" s="11">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J20" s="15">
         <v>7.6150000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>22</v>
       </c>
@@ -1339,14 +2121,15 @@
       <c r="H21" s="8">
         <v>25</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="11">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J21" s="13">
         <v>8.0850000000000009</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1371,7 +2154,8 @@
       <c r="H22" s="2">
         <v>26</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="11">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J22" s="14">
@@ -1403,15 +2187,413 @@
       <c r="H23" s="5">
         <v>26</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23" s="11">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J23" s="15">
         <v>8.0850000000000009</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="18">
+        <v>60.1</v>
+      </c>
+      <c r="G24" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
+        <v>26</v>
+      </c>
+      <c r="I24" s="11">
+        <f>IF(F24&gt;40, 2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="J24" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="17">
+        <v>54.2</v>
+      </c>
+      <c r="G25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2">
+        <v>26</v>
+      </c>
+      <c r="I25" s="11">
+        <f t="shared" ref="I25:I29" si="1">IF(F25&gt;40, 2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="J25" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="17">
+        <v>52.6</v>
+      </c>
+      <c r="G26" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2">
+        <v>26</v>
+      </c>
+      <c r="I26" s="11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J26" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="17">
+        <v>46</v>
+      </c>
+      <c r="G27" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2">
+        <v>26</v>
+      </c>
+      <c r="I27" s="11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J27" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="17">
+        <v>53.3</v>
+      </c>
+      <c r="G28" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2">
+        <v>26</v>
+      </c>
+      <c r="I28" s="11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J28" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="18">
+        <v>45.7</v>
+      </c>
+      <c r="G29" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2">
+        <v>26</v>
+      </c>
+      <c r="I29" s="11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J29" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="17">
+        <v>4.1665999999999999</v>
+      </c>
+      <c r="G30" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2">
+        <v>26</v>
+      </c>
+      <c r="I30" s="11">
+        <f t="shared" ref="I3:I36" si="2">IF(F30&gt;15, 1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="17">
+        <v>4.5454999999999997</v>
+      </c>
+      <c r="G31" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" s="2">
+        <v>26</v>
+      </c>
+      <c r="I31" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+      <c r="F32" s="17">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" s="2">
+        <v>26</v>
+      </c>
+      <c r="I32" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="17">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" s="2">
+        <v>26</v>
+      </c>
+      <c r="I33" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+      <c r="F34" s="17">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" s="2">
+        <v>26</v>
+      </c>
+      <c r="I34" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="17">
+        <v>16.29</v>
+      </c>
+      <c r="I35" s="11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J35" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0</v>
+      </c>
+      <c r="F36" s="17">
+        <v>56.12</v>
+      </c>
+      <c r="I36" s="11">
+        <f>IF(F36&gt;40, 2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="J36" s="14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>